<commit_message>
faculty and request creation completed
</commit_message>
<xml_diff>
--- a/data/faculties.xlsx
+++ b/data/faculties.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -567,27 +567,101 @@
           <t>tambaram,chennai</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="L2" t="n">
+        <v>638057</v>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>chennai</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="O2" t="n">
+        <v>9876543210</v>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>https://google.com/</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>14</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>man</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Doe</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>hello@gmail.com</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Under Graduate</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>SOftware dev</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>aws</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Chennai</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>https://linkedin.com/in/dharunap</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>tambaram,chennai</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
         <is>
           <t>638057</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>chennai</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>India</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="O3" t="inlineStr">
         <is>
           <t>9876543210</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>https://google.com/</t>
         </is>

</xml_diff>